<commit_message>
feat: update manual gene list
</commit_message>
<xml_diff>
--- a/data/manual/manual_gene-list.xlsx
+++ b/data/manual/manual_gene-list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{44B6109E-135F-4F4D-A35F-083CD258FE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8584C94B-5F2F-452F-AE9C-8CFD26F1FD18}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABAA232-F375-4A16-887C-0DE2FB256B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-255" windowWidth="38640" windowHeight="21120" xr2:uid="{C95C6FED-A9B1-47B9-B1E7-71E7CD4356DD}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C95C6FED-A9B1-47B9-B1E7-71E7CD4356DD}"/>
   </bookViews>
   <sheets>
     <sheet name="genes" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="90">
   <si>
     <t>reason</t>
   </si>
@@ -127,6 +127,183 @@
   </si>
   <si>
     <t>2023-06-14</t>
+  </si>
+  <si>
+    <t>ATP7B</t>
+  </si>
+  <si>
+    <t>Wilson disease (OMIM #277900; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>PAH</t>
+  </si>
+  <si>
+    <t>G6PC</t>
+  </si>
+  <si>
+    <t>Glycogen storage disease Ia (OMIM #232200; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>2025-06-19</t>
+  </si>
+  <si>
+    <t>Phenylketonuria (OMIM #261600; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>HEXA</t>
+  </si>
+  <si>
+    <t>ACVRL1</t>
+  </si>
+  <si>
+    <t>ENG</t>
+  </si>
+  <si>
+    <t>NOTCH3</t>
+  </si>
+  <si>
+    <t>TREX1</t>
+  </si>
+  <si>
+    <t>KCNE1</t>
+  </si>
+  <si>
+    <t>KCNQ1</t>
+  </si>
+  <si>
+    <t>LEMD3</t>
+  </si>
+  <si>
+    <t>UBA1</t>
+  </si>
+  <si>
+    <t>CASR</t>
+  </si>
+  <si>
+    <t>ALPL</t>
+  </si>
+  <si>
+    <t>TSHR</t>
+  </si>
+  <si>
+    <t>MEFV</t>
+  </si>
+  <si>
+    <t>C9ORF72</t>
+  </si>
+  <si>
+    <t>FUS</t>
+  </si>
+  <si>
+    <t>TARDBP</t>
+  </si>
+  <si>
+    <t>SOD1</t>
+  </si>
+  <si>
+    <t>GBA</t>
+  </si>
+  <si>
+    <t>LRRK2</t>
+  </si>
+  <si>
+    <t>GRN</t>
+  </si>
+  <si>
+    <t>MAPT</t>
+  </si>
+  <si>
+    <t>PSEN1</t>
+  </si>
+  <si>
+    <t>PSEN2</t>
+  </si>
+  <si>
+    <t>APP</t>
+  </si>
+  <si>
+    <t>DCTN1</t>
+  </si>
+  <si>
+    <t>Tay-Sachs disease (OMIM #272800; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Telangiectasia, hereditary hemorrhagic, type 2 (OMIM #600376; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Telangiectasia, hereditary hemorrhagic, type 1 (OMIM #187300; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Cerebral arteriopathy with subcortical infarcts and leukoencephalopathy 1 (OMIM #125310; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Aicardi-Goutieres syndrome 1, dominant and recessive (OMIM #225750; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Long QT syndrome 5 (OMIM #613695; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Long QT syndrome 1 (OMIM #192500; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Osteopoikilosis with or without melorheostosis (OMIM #166700; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>VEXAS syndrome, somatic (OMIM #	301054; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Hypocalciuric hypercalcemia, type I (OMIM #	145980; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Hypophosphatasia, adult (OMIM #146300; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Hyperthyroidism, nonautoimmune (OMIM #609152; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>MUC1</t>
+  </si>
+  <si>
+    <t>Familial Mediterranean fever, AR (OMIM #249100; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Frontotemporal dementia and/or amyotrophic lateral sclerosis 1 (OMIM #105550; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Amyotrophic lateral sclerosis 6, with or without frontotemporal dementia (OMIM #608030; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Amyotrophic lateral sclerosis 10, with or without FTD (OMIM #612069; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Amyotrophic lateral sclerosis 1 (OMIM #105400; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Tubulointerstitial kidney disease, autosomal dominant, 2 (OMIM #174000; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Gaucher disease, type I (OMIM #230800; frequent diagnostics in Desden)</t>
+  </si>
+  <si>
+    <t>{Parkinson disease 8} (OMIM #607060; frequent diagnostics in Desden)</t>
+  </si>
+  <si>
+    <t>Frontotemporal dementia 2 (OMIM #607485; frequent diagnostics in Desden)</t>
+  </si>
+  <si>
+    <t>Frontotemporal dementia 1, with or without parkinsonism (OMIM #600274; frequent diagnostics in Desden)</t>
+  </si>
+  <si>
+    <t>Dementia, frontotemporal (OMIM #600274; frequent diagnostics in Desden)</t>
+  </si>
+  <si>
+    <t>Alzheimer disease-4 (OMIM #606889; frequent diagnostics in Desden)</t>
+  </si>
+  <si>
+    <t>Cerebral amyloid angiopathy, Dutch, Italian, Iowa, Flemish, Arctic variants (OMIM #605714; frequent diagnostics in Desden)</t>
+  </si>
+  <si>
+    <t>Neuronopathy, distal hereditary motor, autosomal dominant 14 (OMIM #607641; frequent diagnostics in Desden)</t>
   </si>
 </sst>
 </file>
@@ -199,7 +376,18 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -213,9 +401,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -253,7 +441,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -359,7 +547,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -501,7 +689,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -509,7 +697,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D97DC75-4AFF-4124-947F-DBD8EE548F59}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -519,7 +707,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.42578125" style="3"/>
-    <col min="3" max="3" width="102.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="115.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="4"/>
     <col min="6" max="16384" width="11.42578125" style="3"/>
@@ -746,9 +934,505 @@
         <v>30</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E13" xr:uid="{7D97DC75-4AFF-4124-947F-DBD8EE548F59}"/>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
chore: update manual gene list according to mails
</commit_message>
<xml_diff>
--- a/data/manual/manual_gene-list.xlsx
+++ b/data/manual/manual_gene-list.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABAA232-F375-4A16-887C-0DE2FB256B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42D74DC-3293-4637-98A0-C39ED4A9C0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C95C6FED-A9B1-47B9-B1E7-71E7CD4356DD}"/>
   </bookViews>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">genes!$A$1:$E$13</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="188">
   <si>
     <t>reason</t>
   </si>
@@ -304,6 +304,300 @@
   </si>
   <si>
     <t>Neuronopathy, distal hereditary motor, autosomal dominant 14 (OMIM #607641; frequent diagnostics in Desden)</t>
+  </si>
+  <si>
+    <t>DLST</t>
+  </si>
+  <si>
+    <t>EPAS1</t>
+  </si>
+  <si>
+    <t>SLC25A11</t>
+  </si>
+  <si>
+    <t>Pheochromocytoma/paraganglioma syndrome 7 (OMIM #618475; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>GeneReview (Hereditary Paraganglioma-Pheochromocytoma Syndromes; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>Pheochromocytoma/paraganglioma syndrome 6 (OMIM #618464; frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>2025-07-15</t>
+  </si>
+  <si>
+    <t>RAD50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRAXAS1 </t>
+  </si>
+  <si>
+    <t>FBREK consortium research gene</t>
+  </si>
+  <si>
+    <t>TPM1</t>
+  </si>
+  <si>
+    <t>ACMG SF</t>
+  </si>
+  <si>
+    <t>COL3A1</t>
+  </si>
+  <si>
+    <t>ABCD1</t>
+  </si>
+  <si>
+    <t>ACMG SF v3.3</t>
+  </si>
+  <si>
+    <t>CYP27A1</t>
+  </si>
+  <si>
+    <t>PLN</t>
+  </si>
+  <si>
+    <t>ASPH</t>
+  </si>
+  <si>
+    <t>malignant hyperthermia (frequent diagnostics in Leipzig)</t>
+  </si>
+  <si>
+    <t>ATP2A1</t>
+  </si>
+  <si>
+    <t>TRPV1</t>
+  </si>
+  <si>
+    <t>ABCG5</t>
+  </si>
+  <si>
+    <t>hypercholesterolemia (frequent diagnostics in Leipzig)</t>
+  </si>
+  <si>
+    <t>ABCG8</t>
+  </si>
+  <si>
+    <t>LIPA</t>
+  </si>
+  <si>
+    <t>LPL</t>
+  </si>
+  <si>
+    <t>CAV3</t>
+  </si>
+  <si>
+    <t>CETP</t>
+  </si>
+  <si>
+    <t>APOA5</t>
+  </si>
+  <si>
+    <t>hypertriglyceridemia (frequent diagnostics in Leipzig)</t>
+  </si>
+  <si>
+    <t>APOC2</t>
+  </si>
+  <si>
+    <t>CREB3L3</t>
+  </si>
+  <si>
+    <t>GPD1</t>
+  </si>
+  <si>
+    <t>GPIHBP1</t>
+  </si>
+  <si>
+    <t>LMF1</t>
+  </si>
+  <si>
+    <t>CAV1</t>
+  </si>
+  <si>
+    <t>PPARG</t>
+  </si>
+  <si>
+    <t>NPC1L1</t>
+  </si>
+  <si>
+    <t>SORT1</t>
+  </si>
+  <si>
+    <t>STAP1</t>
+  </si>
+  <si>
+    <t>LRP6</t>
+  </si>
+  <si>
+    <t>SCARB1</t>
+  </si>
+  <si>
+    <t>LIPC</t>
+  </si>
+  <si>
+    <t>EPHX2</t>
+  </si>
+  <si>
+    <t>APOA2</t>
+  </si>
+  <si>
+    <t>ABCA1</t>
+  </si>
+  <si>
+    <t>ACADM</t>
+  </si>
+  <si>
+    <t>ACADS</t>
+  </si>
+  <si>
+    <t>ACADVL</t>
+  </si>
+  <si>
+    <t>AGPAT2</t>
+  </si>
+  <si>
+    <t>AKT2</t>
+  </si>
+  <si>
+    <t>ALMS1</t>
+  </si>
+  <si>
+    <t>AMPD1</t>
+  </si>
+  <si>
+    <t>ANGPTL3</t>
+  </si>
+  <si>
+    <t>ANGPTL4</t>
+  </si>
+  <si>
+    <t>APOA1</t>
+  </si>
+  <si>
+    <t>APOA4</t>
+  </si>
+  <si>
+    <t>APOC3</t>
+  </si>
+  <si>
+    <t>BANF1</t>
+  </si>
+  <si>
+    <t>BSCL2</t>
+  </si>
+  <si>
+    <t>CAVIN1</t>
+  </si>
+  <si>
+    <t>CIDEC</t>
+  </si>
+  <si>
+    <t>COQ2</t>
+  </si>
+  <si>
+    <t>CPT2</t>
+  </si>
+  <si>
+    <t>CYP2D6</t>
+  </si>
+  <si>
+    <t>DHCR24</t>
+  </si>
+  <si>
+    <t>DHCR7</t>
+  </si>
+  <si>
+    <t>FBN1</t>
+  </si>
+  <si>
+    <t>GK</t>
+  </si>
+  <si>
+    <t>KCNJ6</t>
+  </si>
+  <si>
+    <t>LCAT</t>
+  </si>
+  <si>
+    <t>LEP</t>
+  </si>
+  <si>
+    <t>LIPE</t>
+  </si>
+  <si>
+    <t>LIPG</t>
+  </si>
+  <si>
+    <t>LMNA</t>
+  </si>
+  <si>
+    <t>LPA</t>
+  </si>
+  <si>
+    <t>LPIN1</t>
+  </si>
+  <si>
+    <t>MTTP</t>
+  </si>
+  <si>
+    <t>NPC1</t>
+  </si>
+  <si>
+    <t>NPC2</t>
+  </si>
+  <si>
+    <t>PCYT1A</t>
+  </si>
+  <si>
+    <t>PDIA2</t>
+  </si>
+  <si>
+    <t>PIK3R1</t>
+  </si>
+  <si>
+    <t>PLIN1</t>
+  </si>
+  <si>
+    <t>POLD1</t>
+  </si>
+  <si>
+    <t>PPARA</t>
+  </si>
+  <si>
+    <t>PRKAA2</t>
+  </si>
+  <si>
+    <t>PSMB8</t>
+  </si>
+  <si>
+    <t>PYGM</t>
+  </si>
+  <si>
+    <t>SAR1B</t>
+  </si>
+  <si>
+    <t>SLC22A8</t>
+  </si>
+  <si>
+    <t>SLCO1B1</t>
+  </si>
+  <si>
+    <t>SMPD1</t>
+  </si>
+  <si>
+    <t>USF1</t>
+  </si>
+  <si>
+    <t>WRN</t>
+  </si>
+  <si>
+    <t>ZMPSTE24</t>
+  </si>
+  <si>
+    <t>hypercholesterolemia risk factor (frequent diagnostics in Leipzig)</t>
+  </si>
+  <si>
+    <t>lipid disorders (frequent diagnostics in Berlin)</t>
   </si>
 </sst>
 </file>
@@ -338,12 +632,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -358,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -372,11 +672,34 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -697,11 +1020,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D97DC75-4AFF-4124-947F-DBD8EE548F59}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1427,11 +1750,1475 @@
         <v>36</v>
       </c>
     </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>42</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>47</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>51</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>52</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>53</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>54</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>55</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>56</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>57</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>58</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>59</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>60</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>61</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>62</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <v>63</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
+        <v>64</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>65</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>66</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
+        <v>67</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
+        <v>68</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <v>69</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <v>70</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <v>71</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <v>72</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
+        <v>73</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
+        <v>74</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <v>75</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
+        <v>76</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <v>77</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <v>78</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="3">
+        <v>79</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="3">
+        <v>80</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="3">
+        <v>81</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
+        <v>82</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
+        <v>83</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
+        <v>84</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="3">
+        <v>85</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="3">
+        <v>86</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="3">
+        <v>87</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="3">
+        <v>88</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="3">
+        <v>89</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="3">
+        <v>90</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="3">
+        <v>91</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="3">
+        <v>92</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="3">
+        <v>93</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="3">
+        <v>94</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="3">
+        <v>95</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="3">
+        <v>96</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="3">
+        <v>97</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="3">
+        <v>98</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="3">
+        <v>99</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="3">
+        <v>100</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="3">
+        <v>101</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="3">
+        <v>102</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="3">
+        <v>103</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="3">
+        <v>104</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="3">
+        <v>105</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="3">
+        <v>106</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="3">
+        <v>107</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="3">
+        <v>108</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="3">
+        <v>109</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="3">
+        <v>110</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="3">
+        <v>111</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="3">
+        <v>112</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="3">
+        <v>113</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="3">
+        <v>114</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="3">
+        <v>115</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="3">
+        <v>116</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E117" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="3">
+        <v>117</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E118" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="3">
+        <v>118</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E119" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="3">
+        <v>119</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E120" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="3">
+        <v>120</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="3">
+        <v>121</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E122" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="3">
+        <v>122</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E123" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="3">
+        <v>123</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="3">
+        <v>124</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E125" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="3">
+        <v>125</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E126" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="3">
+        <v>126</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="3">
+        <v>127</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E13" xr:uid="{7D97DC75-4AFF-4124-947F-DBD8EE548F59}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: add Dresden veto gene list
</commit_message>
<xml_diff>
--- a/data/manual/manual_gene-list.xlsx
+++ b/data/manual/manual_gene-list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42D74DC-3293-4637-98A0-C39ED4A9C0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479EE101-1622-493C-8786-7F0D3A8817E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C95C6FED-A9B1-47B9-B1E7-71E7CD4356DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C95C6FED-A9B1-47B9-B1E7-71E7CD4356DD}"/>
   </bookViews>
   <sheets>
     <sheet name="genes" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="218">
   <si>
     <t>reason</t>
   </si>
@@ -598,6 +598,96 @@
   </si>
   <si>
     <t>lipid disorders (frequent diagnostics in Berlin)</t>
+  </si>
+  <si>
+    <t>IKZF1</t>
+  </si>
+  <si>
+    <t>EZH2</t>
+  </si>
+  <si>
+    <t>BIK</t>
+  </si>
+  <si>
+    <t>CMTR2</t>
+  </si>
+  <si>
+    <t>ATG12</t>
+  </si>
+  <si>
+    <t>FAS</t>
+  </si>
+  <si>
+    <t>RPS24</t>
+  </si>
+  <si>
+    <t>RPS26</t>
+  </si>
+  <si>
+    <t>CREBBP</t>
+  </si>
+  <si>
+    <t>HAVCR2</t>
+  </si>
+  <si>
+    <t>TBXT</t>
+  </si>
+  <si>
+    <t>GJB2</t>
+  </si>
+  <si>
+    <t>HMBS</t>
+  </si>
+  <si>
+    <t>ELP1</t>
+  </si>
+  <si>
+    <t>ERCC6L2</t>
+  </si>
+  <si>
+    <t>GPR161</t>
+  </si>
+  <si>
+    <t>GPR101</t>
+  </si>
+  <si>
+    <t>FLT3</t>
+  </si>
+  <si>
+    <t>HPS1</t>
+  </si>
+  <si>
+    <t>BPTF</t>
+  </si>
+  <si>
+    <t>MNX1</t>
+  </si>
+  <si>
+    <t>MECOM</t>
+  </si>
+  <si>
+    <t>CTLA4</t>
+  </si>
+  <si>
+    <t>ARMC5</t>
+  </si>
+  <si>
+    <t>DROSHA</t>
+  </si>
+  <si>
+    <t>EGLN2</t>
+  </si>
+  <si>
+    <t>NSD1</t>
+  </si>
+  <si>
+    <t>EGLN1</t>
+  </si>
+  <si>
+    <t>cancer risk (Dresden)</t>
+  </si>
+  <si>
+    <t>2025-08-19</t>
   </si>
 </sst>
 </file>
@@ -632,18 +722,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -658,7 +742,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -672,14 +756,57 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1020,11 +1147,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D97DC75-4AFF-4124-947F-DBD8EE548F59}">
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C70" sqref="C70"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1275,1950 +1402,2427 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="D15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="D16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="D17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="D18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="D19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="D20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="D21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="4" t="s">
+      <c r="D22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="4" t="s">
+      <c r="D23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="4" t="s">
+      <c r="D24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="4" t="s">
+      <c r="D25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="D26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="4" t="s">
+      <c r="D27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="4" t="s">
+      <c r="D28" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>28</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E29" s="4" t="s">
+      <c r="D29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
+      <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="4" t="s">
+      <c r="D30" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="4" t="s">
+      <c r="D31" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+      <c r="A32" s="5">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E32" s="4" t="s">
+      <c r="D32" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
+      <c r="A33" s="5">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="4" t="s">
+      <c r="D33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
+      <c r="A34" s="5">
         <v>33</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="4" t="s">
+      <c r="D34" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
+      <c r="A35" s="5">
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" s="4" t="s">
+      <c r="D35" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
+      <c r="A36" s="5">
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E36" s="4" t="s">
+      <c r="D36" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
+      <c r="A37" s="5">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E37" s="4" t="s">
+      <c r="D37" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
+      <c r="A38" s="5">
         <v>37</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38" s="4" t="s">
+      <c r="D38" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
+      <c r="A39" s="5">
         <v>38</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E39" s="4" t="s">
+      <c r="D39" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
+      <c r="A40" s="5">
         <v>39</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E40" s="4" t="s">
+      <c r="D40" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
+      <c r="A41" s="5">
         <v>40</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E41" s="4" t="s">
+      <c r="D41" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
+      <c r="A42" s="5">
         <v>41</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E42" s="4" t="s">
+      <c r="D42" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
+      <c r="A43" s="5">
         <v>42</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E43" s="4" t="s">
+      <c r="D43" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
+      <c r="A44" s="5">
         <v>43</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E44" s="4" t="s">
+      <c r="D44" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
+      <c r="A45" s="5">
         <v>44</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E45" s="4" t="s">
+      <c r="D45" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
+      <c r="A46" s="5">
         <v>45</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E46" s="4" t="s">
+      <c r="D46" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
+      <c r="A47" s="5">
         <v>46</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E47" s="4" t="s">
+      <c r="D47" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E47" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
+      <c r="A48" s="5">
         <v>47</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E48" s="4" t="s">
+      <c r="D48" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
+      <c r="A49" s="5">
         <v>48</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E49" s="4" t="s">
+      <c r="D49" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
+      <c r="A50" s="5">
         <v>49</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E50" s="4" t="s">
+      <c r="D50" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="3">
+      <c r="A51" s="5">
         <v>50</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E51" s="4" t="s">
+      <c r="D51" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
+      <c r="A52" s="5">
         <v>51</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E52" s="4" t="s">
+      <c r="D52" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="3">
+      <c r="A53" s="5">
         <v>52</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E53" s="4" t="s">
+      <c r="D53" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
+      <c r="A54" s="5">
         <v>53</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E54" s="4" t="s">
+      <c r="D54" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="3">
+      <c r="A55" s="5">
         <v>54</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E55" s="4" t="s">
+      <c r="D55" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="3">
+      <c r="A56" s="5">
         <v>55</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E56" s="4" t="s">
+      <c r="D56" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="3">
+      <c r="A57" s="5">
         <v>56</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E57" s="4" t="s">
+      <c r="D57" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="3">
+      <c r="A58" s="5">
         <v>57</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E58" s="4" t="s">
+      <c r="D58" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="3">
+      <c r="A59" s="5">
         <v>58</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E59" s="4" t="s">
+      <c r="D59" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="3">
+      <c r="A60" s="5">
         <v>59</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E60" s="4" t="s">
+      <c r="D60" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E60" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="3">
+      <c r="A61" s="5">
         <v>60</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E61" s="4" t="s">
+      <c r="D61" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E61" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="3">
+      <c r="A62" s="5">
         <v>61</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E62" s="4" t="s">
+      <c r="D62" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="3">
+      <c r="A63" s="5">
         <v>62</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E63" s="4" t="s">
+      <c r="D63" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E63" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="3">
+      <c r="A64" s="5">
         <v>63</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E64" s="4" t="s">
+      <c r="D64" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E64" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="3">
+      <c r="A65" s="5">
         <v>64</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E65" s="4" t="s">
+      <c r="D65" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="3">
+      <c r="A66" s="5">
         <v>65</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E66" s="4" t="s">
+      <c r="D66" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E66" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="3">
+      <c r="A67" s="5">
         <v>66</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E67" s="4" t="s">
+      <c r="D67" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="3">
+      <c r="A68" s="5">
         <v>67</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E68" s="4" t="s">
+      <c r="D68" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E68" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="3">
+      <c r="A69" s="5">
         <v>68</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C69" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E69" s="4" t="s">
+      <c r="D69" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E69" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="3">
+      <c r="A70" s="5">
         <v>69</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="5" t="s">
         <v>127</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E70" s="4" t="s">
+      <c r="D70" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E70" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="3">
+      <c r="A71" s="5">
         <v>70</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="5" t="s">
         <v>128</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D71" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E71" s="4" t="s">
+      <c r="D71" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="3">
+      <c r="A72" s="5">
         <v>71</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="5" t="s">
         <v>129</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E72" s="4" t="s">
+      <c r="D72" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="3">
+      <c r="A73" s="5">
         <v>72</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="5" t="s">
         <v>130</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D73" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E73" s="4" t="s">
+      <c r="D73" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E73" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="3">
+      <c r="A74" s="5">
         <v>73</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="5" t="s">
         <v>131</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E74" s="4" t="s">
+      <c r="D74" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E74" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="3">
+      <c r="A75" s="5">
         <v>74</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="5" t="s">
         <v>132</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D75" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E75" s="4" t="s">
+      <c r="D75" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E75" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="3">
+      <c r="A76" s="5">
         <v>75</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="5" t="s">
         <v>133</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D76" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E76" s="4" t="s">
+      <c r="D76" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E76" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="3">
+      <c r="A77" s="5">
         <v>76</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="5" t="s">
         <v>134</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D77" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E77" s="4" t="s">
+      <c r="D77" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E77" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="3">
+      <c r="A78" s="5">
         <v>77</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="5" t="s">
         <v>135</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D78" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E78" s="4" t="s">
+      <c r="D78" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E78" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="3">
+      <c r="A79" s="5">
         <v>78</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="5" t="s">
         <v>136</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D79" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E79" s="4" t="s">
+      <c r="D79" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="3">
+      <c r="A80" s="5">
         <v>79</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="5" t="s">
         <v>137</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D80" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E80" s="4" t="s">
+      <c r="D80" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E80" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="3">
+      <c r="A81" s="5">
         <v>80</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="5" t="s">
         <v>138</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D81" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E81" s="4" t="s">
+      <c r="D81" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E81" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="3">
+      <c r="A82" s="5">
         <v>81</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="5" t="s">
         <v>139</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D82" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E82" s="4" t="s">
+      <c r="D82" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E82" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="3">
+      <c r="A83" s="5">
         <v>82</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="5" t="s">
         <v>140</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D83" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E83" s="4" t="s">
+      <c r="D83" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E83" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="3">
+      <c r="A84" s="5">
         <v>83</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="5" t="s">
         <v>141</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E84" s="4" t="s">
+      <c r="D84" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E84" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="3">
+      <c r="A85" s="5">
         <v>84</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="5" t="s">
         <v>142</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D85" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E85" s="4" t="s">
+      <c r="D85" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E85" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="3">
+      <c r="A86" s="5">
         <v>85</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="5" t="s">
         <v>143</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E86" s="4" t="s">
+      <c r="D86" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E86" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="3">
+      <c r="A87" s="5">
         <v>86</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="5" t="s">
         <v>144</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D87" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E87" s="4" t="s">
+      <c r="D87" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E87" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="3">
+      <c r="A88" s="5">
         <v>87</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="5" t="s">
         <v>145</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D88" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E88" s="4" t="s">
+      <c r="D88" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E88" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="3">
+      <c r="A89" s="5">
         <v>88</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="5" t="s">
         <v>146</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D89" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E89" s="4" t="s">
+      <c r="D89" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E89" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="3">
+      <c r="A90" s="5">
         <v>89</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="5" t="s">
         <v>147</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D90" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E90" s="4" t="s">
+      <c r="D90" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E90" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="3">
+      <c r="A91" s="5">
         <v>90</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="5" t="s">
         <v>148</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D91" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E91" s="4" t="s">
+      <c r="D91" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E91" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="3">
+      <c r="A92" s="5">
         <v>91</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="5" t="s">
         <v>149</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D92" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E92" s="4" t="s">
+      <c r="D92" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E92" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="3">
+      <c r="A93" s="5">
         <v>92</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="5" t="s">
         <v>150</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E93" s="4" t="s">
+      <c r="D93" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E93" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="3">
+      <c r="A94" s="5">
         <v>93</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="5" t="s">
         <v>151</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D94" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E94" s="4" t="s">
+      <c r="D94" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E94" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="3">
+      <c r="A95" s="5">
         <v>94</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="5" t="s">
         <v>152</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D95" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E95" s="4" t="s">
+      <c r="D95" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E95" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="3">
+      <c r="A96" s="5">
         <v>95</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="5" t="s">
         <v>153</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D96" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E96" s="4" t="s">
+      <c r="D96" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E96" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="3">
-        <v>96</v>
-      </c>
-      <c r="B97" s="3" t="s">
+      <c r="A97" s="5">
+        <v>96</v>
+      </c>
+      <c r="B97" s="5" t="s">
         <v>154</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D97" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E97" s="4" t="s">
+      <c r="D97" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E97" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="3">
+      <c r="A98" s="5">
         <v>97</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B98" s="5" t="s">
         <v>155</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D98" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E98" s="4" t="s">
+      <c r="D98" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E98" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="3">
+      <c r="A99" s="5">
         <v>98</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B99" s="5" t="s">
         <v>156</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E99" s="4" t="s">
+      <c r="D99" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E99" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="3">
+      <c r="A100" s="5">
         <v>99</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B100" s="5" t="s">
         <v>157</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D100" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E100" s="4" t="s">
+      <c r="D100" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E100" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="3">
+      <c r="A101" s="5">
         <v>100</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B101" s="5" t="s">
         <v>158</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D101" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E101" s="4" t="s">
+      <c r="D101" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E101" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="3">
+      <c r="A102" s="5">
         <v>101</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B102" s="5" t="s">
         <v>159</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D102" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E102" s="4" t="s">
+      <c r="D102" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E102" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="3">
+      <c r="A103" s="5">
         <v>102</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B103" s="5" t="s">
         <v>160</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D103" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E103" s="4" t="s">
+      <c r="D103" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E103" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="3">
+      <c r="A104" s="5">
         <v>103</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B104" s="5" t="s">
         <v>161</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D104" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E104" s="4" t="s">
+      <c r="D104" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E104" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="3">
+      <c r="A105" s="5">
         <v>104</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B105" s="5" t="s">
         <v>162</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D105" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E105" s="4" t="s">
+      <c r="D105" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E105" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="3">
+      <c r="A106" s="5">
         <v>105</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="5" t="s">
         <v>163</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D106" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E106" s="4" t="s">
+      <c r="D106" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E106" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="3">
+      <c r="A107" s="5">
         <v>106</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B107" s="5" t="s">
         <v>164</v>
       </c>
       <c r="C107" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D107" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E107" s="4" t="s">
+      <c r="D107" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E107" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="3">
+      <c r="A108" s="5">
         <v>107</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B108" s="5" t="s">
         <v>165</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D108" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E108" s="4" t="s">
+      <c r="D108" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E108" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="3">
+      <c r="A109" s="5">
         <v>108</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B109" s="5" t="s">
         <v>166</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D109" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E109" s="4" t="s">
+      <c r="D109" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E109" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="3">
+      <c r="A110" s="5">
         <v>109</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B110" s="5" t="s">
         <v>167</v>
       </c>
       <c r="C110" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D110" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E110" s="4" t="s">
+      <c r="D110" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E110" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="3">
+      <c r="A111" s="5">
         <v>110</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B111" s="5" t="s">
         <v>168</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D111" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E111" s="4" t="s">
+      <c r="D111" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E111" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="3">
+      <c r="A112" s="5">
         <v>111</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B112" s="5" t="s">
         <v>169</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D112" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E112" s="4" t="s">
+      <c r="D112" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E112" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="3">
+      <c r="A113" s="5">
         <v>112</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" s="5" t="s">
         <v>170</v>
       </c>
       <c r="C113" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D113" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E113" s="4" t="s">
+      <c r="D113" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E113" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="3">
+      <c r="A114" s="5">
         <v>113</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B114" s="5" t="s">
         <v>171</v>
       </c>
       <c r="C114" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D114" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E114" s="4" t="s">
+      <c r="D114" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E114" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="3">
+      <c r="A115" s="5">
         <v>114</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B115" s="5" t="s">
         <v>172</v>
       </c>
       <c r="C115" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D115" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E115" s="4" t="s">
+      <c r="D115" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E115" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="3">
+      <c r="A116" s="5">
         <v>115</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B116" s="5" t="s">
         <v>173</v>
       </c>
       <c r="C116" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D116" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E116" s="4" t="s">
+      <c r="D116" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E116" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="3">
+      <c r="A117" s="5">
         <v>116</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B117" s="5" t="s">
         <v>174</v>
       </c>
       <c r="C117" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D117" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E117" s="4" t="s">
+      <c r="D117" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E117" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="3">
+      <c r="A118" s="5">
         <v>117</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B118" s="5" t="s">
         <v>175</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D118" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E118" s="4" t="s">
+      <c r="D118" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E118" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="3">
+      <c r="A119" s="5">
         <v>118</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B119" s="5" t="s">
         <v>176</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D119" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E119" s="4" t="s">
+      <c r="D119" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E119" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="3">
+      <c r="A120" s="5">
         <v>119</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B120" s="5" t="s">
         <v>177</v>
       </c>
       <c r="C120" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D120" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E120" s="4" t="s">
+      <c r="D120" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E120" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="3">
+      <c r="A121" s="5">
         <v>120</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B121" s="5" t="s">
         <v>178</v>
       </c>
       <c r="C121" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D121" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E121" s="4" t="s">
+      <c r="D121" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E121" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="3">
+      <c r="A122" s="5">
         <v>121</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B122" s="5" t="s">
         <v>179</v>
       </c>
       <c r="C122" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D122" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E122" s="4" t="s">
+      <c r="D122" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E122" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="3">
+      <c r="A123" s="5">
         <v>122</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="B123" s="5" t="s">
         <v>180</v>
       </c>
       <c r="C123" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D123" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E123" s="4" t="s">
+      <c r="D123" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E123" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="3">
+      <c r="A124" s="5">
         <v>123</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B124" s="5" t="s">
         <v>181</v>
       </c>
       <c r="C124" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D124" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E124" s="4" t="s">
+      <c r="D124" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E124" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="3">
+      <c r="A125" s="5">
         <v>124</v>
       </c>
-      <c r="B125" s="3" t="s">
+      <c r="B125" s="5" t="s">
         <v>182</v>
       </c>
       <c r="C125" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D125" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E125" s="4" t="s">
+      <c r="D125" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E125" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="3">
+      <c r="A126" s="5">
         <v>125</v>
       </c>
-      <c r="B126" s="3" t="s">
+      <c r="B126" s="5" t="s">
         <v>183</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D126" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E126" s="4" t="s">
+      <c r="D126" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E126" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="3">
+      <c r="A127" s="5">
         <v>126</v>
       </c>
-      <c r="B127" s="3" t="s">
+      <c r="B127" s="5" t="s">
         <v>184</v>
       </c>
       <c r="C127" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D127" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E127" s="4" t="s">
+      <c r="D127" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E127" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="3">
+      <c r="A128" s="5">
         <v>127</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="B128" s="5" t="s">
         <v>185</v>
       </c>
       <c r="C128" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D128" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E128" s="4" t="s">
-        <v>96</v>
+      <c r="D128" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E128" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="5">
+        <v>128</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D129" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E129" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="5">
+        <v>129</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D130" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E130" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="5">
+        <v>130</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D131" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E131" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="5">
+        <v>131</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E132" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="5">
+        <v>132</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E133" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="5">
+        <v>133</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E134" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="5">
+        <v>134</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E135" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="5">
+        <v>135</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E136" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="5">
+        <v>136</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D137" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E137" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="5">
+        <v>137</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E138" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="5">
+        <v>138</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C139" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D139" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E139" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="5">
+        <v>139</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D140" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E140" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="5">
+        <v>140</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D141" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E141" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="5">
+        <v>141</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D142" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E142" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="5">
+        <v>142</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C143" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D143" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E143" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="5">
+        <v>143</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D144" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E144" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="5">
+        <v>144</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D145" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E145" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="5">
+        <v>145</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D146" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E146" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="5">
+        <v>146</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D147" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E147" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="5">
+        <v>147</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D148" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E148" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="5">
+        <v>148</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C149" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D149" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E149" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="5">
+        <v>149</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D150" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E150" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="5">
+        <v>150</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D151" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E151" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="5">
+        <v>151</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D152" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E152" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="5">
+        <v>152</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C153" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D153" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E153" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="5">
+        <v>153</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D154" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E154" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="5">
+        <v>154</v>
+      </c>
+      <c r="B155" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D155" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E155" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="5">
+        <v>155</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C156" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D156" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E156" s="6" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E13" xr:uid="{7D97DC75-4AFF-4124-947F-DBD8EE548F59}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: add SPRTN to veto manual list
</commit_message>
<xml_diff>
--- a/data/manual/manual_gene-list.xlsx
+++ b/data/manual/manual_gene-list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479EE101-1622-493C-8786-7F0D3A8817E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC0A392-E046-4EAC-B591-564A9E60B214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C95C6FED-A9B1-47B9-B1E7-71E7CD4356DD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="220">
   <si>
     <t>reason</t>
   </si>
@@ -688,6 +688,12 @@
   </si>
   <si>
     <t>2025-08-19</t>
+  </si>
+  <si>
+    <t>SPRTN</t>
+  </si>
+  <si>
+    <t>2025-08-21</t>
   </si>
 </sst>
 </file>
@@ -742,7 +748,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -756,47 +762,11 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1147,7 +1117,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D97DC75-4AFF-4124-947F-DBD8EE548F59}">
-  <dimension ref="A1:E156"/>
+  <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1402,2427 +1372,2444 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="6" t="s">
+      <c r="D16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="D17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="D18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="6" t="s">
+      <c r="D19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="6" t="s">
+      <c r="D20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="6" t="s">
+      <c r="D21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="6" t="s">
+      <c r="D22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="6" t="s">
+      <c r="D23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="D24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="6" t="s">
+      <c r="D25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="D26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="6" t="s">
+      <c r="D27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="6" t="s">
+      <c r="D28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>28</v>
-      </c>
-      <c r="B29" s="5" t="s">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E29" s="6" t="s">
+      <c r="D29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="6" t="s">
+      <c r="D30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="6" t="s">
+      <c r="D31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E32" s="6" t="s">
+      <c r="D32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="6" t="s">
+      <c r="D33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="6" t="s">
+      <c r="D34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" s="6" t="s">
+      <c r="D35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E36" s="6" t="s">
+      <c r="D36" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E37" s="6" t="s">
+      <c r="D37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38" s="6" t="s">
+      <c r="D38" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E39" s="6" t="s">
+      <c r="D39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E40" s="6" t="s">
+      <c r="D40" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E41" s="6" t="s">
+      <c r="D41" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E42" s="6" t="s">
+      <c r="D42" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
+      <c r="A43" s="3">
         <v>42</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E43" s="6" t="s">
+      <c r="D43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
+      <c r="A44" s="3">
         <v>43</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E44" s="6" t="s">
+      <c r="D44" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
+      <c r="A45" s="3">
         <v>44</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E45" s="6" t="s">
+      <c r="D45" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
+      <c r="A46" s="3">
         <v>45</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E46" s="6" t="s">
+      <c r="D46" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
+      <c r="A47" s="3">
         <v>46</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E47" s="6" t="s">
+      <c r="D47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
+      <c r="A48" s="3">
         <v>47</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E48" s="6" t="s">
+      <c r="D48" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="5">
+      <c r="A49" s="3">
         <v>48</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E49" s="6" t="s">
+      <c r="D49" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
+      <c r="A50" s="3">
         <v>49</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E50" s="6" t="s">
+      <c r="D50" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="5">
+      <c r="A51" s="3">
         <v>50</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D51" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E51" s="6" t="s">
+      <c r="D51" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="5">
+      <c r="A52" s="3">
         <v>51</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E52" s="6" t="s">
+      <c r="D52" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="5">
+      <c r="A53" s="3">
         <v>52</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E53" s="6" t="s">
+      <c r="D53" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="5">
+      <c r="A54" s="3">
         <v>53</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E54" s="6" t="s">
+      <c r="D54" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="5">
+      <c r="A55" s="3">
         <v>54</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D55" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E55" s="6" t="s">
+      <c r="D55" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="5">
+      <c r="A56" s="3">
         <v>55</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E56" s="6" t="s">
+      <c r="D56" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="5">
+      <c r="A57" s="3">
         <v>56</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E57" s="6" t="s">
+      <c r="D57" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="5">
+      <c r="A58" s="3">
         <v>57</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E58" s="6" t="s">
+      <c r="D58" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="5">
+      <c r="A59" s="3">
         <v>58</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E59" s="6" t="s">
+      <c r="D59" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E59" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="5">
+      <c r="A60" s="3">
         <v>59</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E60" s="6" t="s">
+      <c r="D60" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E60" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
+      <c r="A61" s="3">
         <v>60</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E61" s="6" t="s">
+      <c r="D61" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E61" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="5">
+      <c r="A62" s="3">
         <v>61</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D62" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E62" s="6" t="s">
+      <c r="D62" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="5">
+      <c r="A63" s="3">
         <v>62</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D63" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E63" s="6" t="s">
+      <c r="D63" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E63" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="5">
+      <c r="A64" s="3">
         <v>63</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D64" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E64" s="6" t="s">
+      <c r="D64" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E64" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
+      <c r="A65" s="3">
         <v>64</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E65" s="6" t="s">
+      <c r="D65" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="5">
+      <c r="A66" s="3">
         <v>65</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D66" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E66" s="6" t="s">
+      <c r="D66" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E66" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="5">
+      <c r="A67" s="3">
         <v>66</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D67" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E67" s="6" t="s">
+      <c r="D67" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="5">
+      <c r="A68" s="3">
         <v>67</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D68" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E68" s="6" t="s">
+      <c r="D68" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E68" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="5">
+      <c r="A69" s="3">
         <v>68</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D69" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E69" s="6" t="s">
+      <c r="D69" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E69" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="5">
+      <c r="A70" s="3">
         <v>69</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D70" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E70" s="6" t="s">
+      <c r="D70" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E70" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="5">
+      <c r="A71" s="3">
         <v>70</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C71" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D71" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E71" s="6" t="s">
+      <c r="D71" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="5">
+      <c r="A72" s="3">
         <v>71</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C72" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D72" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E72" s="6" t="s">
+      <c r="D72" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="5">
+      <c r="A73" s="3">
         <v>72</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C73" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D73" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E73" s="6" t="s">
+      <c r="D73" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E73" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="5">
+      <c r="A74" s="3">
         <v>73</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C74" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D74" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E74" s="6" t="s">
+      <c r="D74" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E74" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="5">
+      <c r="A75" s="3">
         <v>74</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C75" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D75" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E75" s="6" t="s">
+      <c r="D75" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E75" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="5">
+      <c r="A76" s="3">
         <v>75</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C76" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D76" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E76" s="6" t="s">
+      <c r="D76" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E76" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="5">
+      <c r="A77" s="3">
         <v>76</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D77" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E77" s="6" t="s">
+      <c r="D77" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E77" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="5">
+      <c r="A78" s="3">
         <v>77</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C78" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E78" s="6" t="s">
+      <c r="C78" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E78" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="5">
+      <c r="A79" s="3">
         <v>78</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C79" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E79" s="6" t="s">
+      <c r="C79" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E79" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="5">
+      <c r="A80" s="3">
         <v>79</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E80" s="6" t="s">
+      <c r="C80" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E80" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="5">
+      <c r="A81" s="3">
         <v>80</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C81" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E81" s="6" t="s">
+      <c r="C81" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E81" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="5">
+      <c r="A82" s="3">
         <v>81</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C82" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E82" s="6" t="s">
+      <c r="C82" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E82" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="5">
+      <c r="A83" s="3">
         <v>82</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C83" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E83" s="6" t="s">
+      <c r="C83" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E83" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="5">
+      <c r="A84" s="3">
         <v>83</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C84" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E84" s="6" t="s">
+      <c r="C84" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E84" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="5">
+      <c r="A85" s="3">
         <v>84</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C85" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E85" s="6" t="s">
+      <c r="C85" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E85" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="5">
+      <c r="A86" s="3">
         <v>85</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C86" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E86" s="6" t="s">
+      <c r="C86" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E86" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="5">
+      <c r="A87" s="3">
         <v>86</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C87" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E87" s="6" t="s">
+      <c r="C87" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E87" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="5">
+      <c r="A88" s="3">
         <v>87</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C88" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E88" s="6" t="s">
+      <c r="C88" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E88" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="5">
+      <c r="A89" s="3">
         <v>88</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C89" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E89" s="6" t="s">
+      <c r="C89" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E89" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="5">
+      <c r="A90" s="3">
         <v>89</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C90" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E90" s="6" t="s">
+      <c r="C90" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E90" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="5">
+      <c r="A91" s="3">
         <v>90</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C91" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E91" s="6" t="s">
+      <c r="C91" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E91" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="5">
+      <c r="A92" s="3">
         <v>91</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C92" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E92" s="6" t="s">
+      <c r="C92" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E92" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="5">
+      <c r="A93" s="3">
         <v>92</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C93" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E93" s="6" t="s">
+      <c r="C93" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E93" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="5">
+      <c r="A94" s="3">
         <v>93</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C94" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D94" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E94" s="6" t="s">
+      <c r="C94" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E94" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="5">
+      <c r="A95" s="3">
         <v>94</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C95" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D95" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E95" s="6" t="s">
+      <c r="C95" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E95" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="5">
+      <c r="A96" s="3">
         <v>95</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C96" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D96" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E96" s="6" t="s">
+      <c r="C96" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E96" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="5">
-        <v>96</v>
-      </c>
-      <c r="B97" s="5" t="s">
+      <c r="A97" s="3">
+        <v>96</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C97" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E97" s="6" t="s">
+      <c r="C97" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E97" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="5">
+      <c r="A98" s="3">
         <v>97</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C98" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E98" s="6" t="s">
+      <c r="C98" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E98" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="5">
+      <c r="A99" s="3">
         <v>98</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C99" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D99" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E99" s="6" t="s">
+      <c r="C99" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E99" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="5">
+      <c r="A100" s="3">
         <v>99</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B100" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C100" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D100" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E100" s="6" t="s">
+      <c r="C100" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E100" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="5">
+      <c r="A101" s="3">
         <v>100</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C101" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E101" s="6" t="s">
+      <c r="C101" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E101" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="5">
+      <c r="A102" s="3">
         <v>101</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C102" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D102" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E102" s="6" t="s">
+      <c r="C102" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E102" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="5">
+      <c r="A103" s="3">
         <v>102</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C103" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E103" s="6" t="s">
+      <c r="C103" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E103" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="5">
+      <c r="A104" s="3">
         <v>103</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B104" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C104" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D104" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E104" s="6" t="s">
+      <c r="C104" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E104" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="5">
+      <c r="A105" s="3">
         <v>104</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="B105" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C105" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E105" s="6" t="s">
+      <c r="C105" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E105" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="5">
+      <c r="A106" s="3">
         <v>105</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C106" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D106" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E106" s="6" t="s">
+      <c r="C106" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E106" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="5">
+      <c r="A107" s="3">
         <v>106</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B107" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C107" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E107" s="6" t="s">
+      <c r="C107" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E107" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="5">
+      <c r="A108" s="3">
         <v>107</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="B108" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C108" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E108" s="6" t="s">
+      <c r="C108" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E108" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="5">
+      <c r="A109" s="3">
         <v>108</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="B109" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C109" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D109" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E109" s="6" t="s">
+      <c r="C109" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E109" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="5">
+      <c r="A110" s="3">
         <v>109</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="B110" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C110" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D110" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E110" s="6" t="s">
+      <c r="C110" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E110" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="5">
+      <c r="A111" s="3">
         <v>110</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="B111" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C111" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E111" s="6" t="s">
+      <c r="C111" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E111" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="5">
+      <c r="A112" s="3">
         <v>111</v>
       </c>
-      <c r="B112" s="5" t="s">
+      <c r="B112" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C112" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D112" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E112" s="6" t="s">
+      <c r="C112" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E112" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="5">
+      <c r="A113" s="3">
         <v>112</v>
       </c>
-      <c r="B113" s="5" t="s">
+      <c r="B113" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C113" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D113" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E113" s="6" t="s">
+      <c r="C113" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E113" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="5">
+      <c r="A114" s="3">
         <v>113</v>
       </c>
-      <c r="B114" s="5" t="s">
+      <c r="B114" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C114" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D114" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E114" s="6" t="s">
+      <c r="C114" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E114" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="5">
+      <c r="A115" s="3">
         <v>114</v>
       </c>
-      <c r="B115" s="5" t="s">
+      <c r="B115" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C115" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D115" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E115" s="6" t="s">
+      <c r="C115" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E115" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="5">
+      <c r="A116" s="3">
         <v>115</v>
       </c>
-      <c r="B116" s="5" t="s">
+      <c r="B116" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C116" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D116" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E116" s="6" t="s">
+      <c r="C116" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E116" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="5">
+      <c r="A117" s="3">
         <v>116</v>
       </c>
-      <c r="B117" s="5" t="s">
+      <c r="B117" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C117" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D117" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E117" s="6" t="s">
+      <c r="C117" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E117" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="5">
+      <c r="A118" s="3">
         <v>117</v>
       </c>
-      <c r="B118" s="5" t="s">
+      <c r="B118" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C118" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D118" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E118" s="6" t="s">
+      <c r="C118" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E118" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="5">
+      <c r="A119" s="3">
         <v>118</v>
       </c>
-      <c r="B119" s="5" t="s">
+      <c r="B119" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C119" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D119" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E119" s="6" t="s">
+      <c r="C119" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E119" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="5">
+      <c r="A120" s="3">
         <v>119</v>
       </c>
-      <c r="B120" s="5" t="s">
+      <c r="B120" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C120" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D120" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E120" s="6" t="s">
+      <c r="C120" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E120" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="5">
+      <c r="A121" s="3">
         <v>120</v>
       </c>
-      <c r="B121" s="5" t="s">
+      <c r="B121" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C121" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D121" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E121" s="6" t="s">
+      <c r="C121" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E121" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="5">
+      <c r="A122" s="3">
         <v>121</v>
       </c>
-      <c r="B122" s="5" t="s">
+      <c r="B122" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C122" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D122" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E122" s="6" t="s">
+      <c r="C122" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E122" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="5">
+      <c r="A123" s="3">
         <v>122</v>
       </c>
-      <c r="B123" s="5" t="s">
+      <c r="B123" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C123" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D123" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E123" s="6" t="s">
+      <c r="C123" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E123" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="5">
+      <c r="A124" s="3">
         <v>123</v>
       </c>
-      <c r="B124" s="5" t="s">
+      <c r="B124" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C124" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D124" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E124" s="6" t="s">
+      <c r="C124" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E124" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="5">
+      <c r="A125" s="3">
         <v>124</v>
       </c>
-      <c r="B125" s="5" t="s">
+      <c r="B125" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C125" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D125" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E125" s="6" t="s">
+      <c r="C125" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E125" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="5">
+      <c r="A126" s="3">
         <v>125</v>
       </c>
-      <c r="B126" s="5" t="s">
+      <c r="B126" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C126" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D126" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E126" s="6" t="s">
+      <c r="C126" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E126" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="5">
+      <c r="A127" s="3">
         <v>126</v>
       </c>
-      <c r="B127" s="5" t="s">
+      <c r="B127" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C127" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D127" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E127" s="6" t="s">
+      <c r="C127" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E127" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="5">
+      <c r="A128" s="3">
         <v>127</v>
       </c>
-      <c r="B128" s="5" t="s">
+      <c r="B128" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C128" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D128" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E128" s="6" t="s">
+      <c r="C128" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E128" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="5">
+      <c r="A129" s="3">
         <v>128</v>
       </c>
-      <c r="B129" s="5" t="s">
+      <c r="B129" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C129" s="5" t="s">
+      <c r="C129" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D129" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E129" s="6" t="s">
+      <c r="D129" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E129" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" s="5">
+      <c r="A130" s="3">
         <v>129</v>
       </c>
-      <c r="B130" s="5" t="s">
+      <c r="B130" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="C130" s="5" t="s">
+      <c r="C130" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D130" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E130" s="6" t="s">
+      <c r="D130" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E130" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" s="5">
+      <c r="A131" s="3">
         <v>130</v>
       </c>
-      <c r="B131" s="5" t="s">
+      <c r="B131" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C131" s="5" t="s">
+      <c r="C131" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D131" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E131" s="6" t="s">
+      <c r="D131" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E131" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="5">
+      <c r="A132" s="3">
         <v>131</v>
       </c>
-      <c r="B132" s="5" t="s">
+      <c r="B132" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C132" s="5" t="s">
+      <c r="C132" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D132" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E132" s="6" t="s">
+      <c r="D132" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E132" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="5">
+      <c r="A133" s="3">
         <v>132</v>
       </c>
-      <c r="B133" s="5" t="s">
+      <c r="B133" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C133" s="5" t="s">
+      <c r="C133" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D133" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E133" s="6" t="s">
+      <c r="D133" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E133" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="5">
+      <c r="A134" s="3">
         <v>133</v>
       </c>
-      <c r="B134" s="5" t="s">
+      <c r="B134" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="C134" s="5" t="s">
+      <c r="C134" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D134" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E134" s="6" t="s">
+      <c r="D134" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E134" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="5">
+      <c r="A135" s="3">
         <v>134</v>
       </c>
-      <c r="B135" s="5" t="s">
+      <c r="B135" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C135" s="5" t="s">
+      <c r="C135" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D135" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E135" s="6" t="s">
+      <c r="D135" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E135" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" s="5">
+      <c r="A136" s="3">
         <v>135</v>
       </c>
-      <c r="B136" s="5" t="s">
+      <c r="B136" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C136" s="5" t="s">
+      <c r="C136" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D136" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E136" s="6" t="s">
+      <c r="D136" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E136" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" s="5">
+      <c r="A137" s="3">
         <v>136</v>
       </c>
-      <c r="B137" s="5" t="s">
+      <c r="B137" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="C137" s="5" t="s">
+      <c r="C137" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D137" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E137" s="6" t="s">
+      <c r="D137" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E137" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" s="5">
+      <c r="A138" s="3">
         <v>137</v>
       </c>
-      <c r="B138" s="5" t="s">
+      <c r="B138" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C138" s="5" t="s">
+      <c r="C138" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D138" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E138" s="6" t="s">
+      <c r="D138" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E138" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" s="5">
+      <c r="A139" s="3">
         <v>138</v>
       </c>
-      <c r="B139" s="5" t="s">
+      <c r="B139" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C139" s="5" t="s">
+      <c r="C139" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D139" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E139" s="6" t="s">
+      <c r="D139" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E139" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" s="5">
+      <c r="A140" s="3">
         <v>139</v>
       </c>
-      <c r="B140" s="5" t="s">
+      <c r="B140" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C140" s="5" t="s">
+      <c r="C140" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D140" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E140" s="6" t="s">
+      <c r="D140" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E140" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" s="5">
+      <c r="A141" s="3">
         <v>140</v>
       </c>
-      <c r="B141" s="5" t="s">
+      <c r="B141" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="C141" s="5" t="s">
+      <c r="C141" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D141" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E141" s="6" t="s">
+      <c r="D141" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E141" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" s="5">
+      <c r="A142" s="3">
         <v>141</v>
       </c>
-      <c r="B142" s="5" t="s">
+      <c r="B142" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C142" s="5" t="s">
+      <c r="C142" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D142" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E142" s="6" t="s">
+      <c r="D142" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E142" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" s="5">
+      <c r="A143" s="3">
         <v>142</v>
       </c>
-      <c r="B143" s="5" t="s">
+      <c r="B143" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C143" s="5" t="s">
+      <c r="C143" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D143" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E143" s="6" t="s">
+      <c r="D143" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E143" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" s="5">
+      <c r="A144" s="3">
         <v>143</v>
       </c>
-      <c r="B144" s="5" t="s">
+      <c r="B144" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C144" s="5" t="s">
+      <c r="C144" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D144" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E144" s="6" t="s">
+      <c r="D144" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E144" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" s="5">
+      <c r="A145" s="3">
         <v>144</v>
       </c>
-      <c r="B145" s="5" t="s">
+      <c r="B145" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C145" s="5" t="s">
+      <c r="C145" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D145" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E145" s="6" t="s">
+      <c r="D145" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E145" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" s="5">
+      <c r="A146" s="3">
         <v>145</v>
       </c>
-      <c r="B146" s="5" t="s">
+      <c r="B146" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C146" s="5" t="s">
+      <c r="C146" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D146" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E146" s="6" t="s">
+      <c r="D146" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E146" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" s="5">
+      <c r="A147" s="3">
         <v>146</v>
       </c>
-      <c r="B147" s="5" t="s">
+      <c r="B147" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C147" s="5" t="s">
+      <c r="C147" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D147" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E147" s="6" t="s">
+      <c r="D147" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E147" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" s="5">
+      <c r="A148" s="3">
         <v>147</v>
       </c>
-      <c r="B148" s="5" t="s">
+      <c r="B148" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C148" s="5" t="s">
+      <c r="C148" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D148" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E148" s="6" t="s">
+      <c r="D148" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E148" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" s="5">
+      <c r="A149" s="3">
         <v>148</v>
       </c>
-      <c r="B149" s="5" t="s">
+      <c r="B149" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C149" s="5" t="s">
+      <c r="C149" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D149" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E149" s="6" t="s">
+      <c r="D149" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E149" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" s="5">
+      <c r="A150" s="3">
         <v>149</v>
       </c>
-      <c r="B150" s="5" t="s">
+      <c r="B150" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C150" s="5" t="s">
+      <c r="C150" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D150" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E150" s="6" t="s">
+      <c r="D150" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E150" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" s="5">
+      <c r="A151" s="3">
         <v>150</v>
       </c>
-      <c r="B151" s="5" t="s">
+      <c r="B151" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C151" s="5" t="s">
+      <c r="C151" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D151" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E151" s="6" t="s">
+      <c r="D151" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E151" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" s="5">
+      <c r="A152" s="3">
         <v>151</v>
       </c>
-      <c r="B152" s="5" t="s">
+      <c r="B152" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C152" s="5" t="s">
+      <c r="C152" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D152" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E152" s="6" t="s">
+      <c r="D152" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E152" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" s="5">
+      <c r="A153" s="3">
         <v>152</v>
       </c>
-      <c r="B153" s="5" t="s">
+      <c r="B153" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C153" s="5" t="s">
+      <c r="C153" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D153" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E153" s="6" t="s">
+      <c r="D153" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E153" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" s="5">
+      <c r="A154" s="3">
         <v>153</v>
       </c>
-      <c r="B154" s="5" t="s">
+      <c r="B154" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C154" s="5" t="s">
+      <c r="C154" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D154" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E154" s="6" t="s">
+      <c r="D154" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E154" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" s="5">
+      <c r="A155" s="3">
         <v>154</v>
       </c>
-      <c r="B155" s="5" t="s">
+      <c r="B155" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C155" s="5" t="s">
+      <c r="C155" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D155" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E155" s="6" t="s">
+      <c r="D155" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E155" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" s="5">
+      <c r="A156" s="3">
         <v>155</v>
       </c>
-      <c r="B156" s="5" t="s">
+      <c r="B156" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="C156" s="5" t="s">
+      <c r="C156" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D156" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E156" s="6" t="s">
+      <c r="D156" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E156" s="4" t="s">
         <v>217</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="3">
+        <v>156</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E157" s="4" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E13" xr:uid="{7D97DC75-4AFF-4124-947F-DBD8EE548F59}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: add missing trusrisk research genes
</commit_message>
<xml_diff>
--- a/data/manual/manual_gene-list.xlsx
+++ b/data/manual/manual_gene-list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A166A5-9547-43E6-9E34-F114E7B89E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8909B715-F61A-4CF8-97AA-06E594AB081F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C95C6FED-A9B1-47B9-B1E7-71E7CD4356DD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="226">
   <si>
     <t>reason</t>
   </si>
@@ -703,6 +703,15 @@
   </si>
   <si>
     <t>2025-09-10</t>
+  </si>
+  <si>
+    <t>MRE11A</t>
+  </si>
+  <si>
+    <t>FAM175A</t>
+  </si>
+  <si>
+    <t>TruRisk v5.0 Genpanel research gene</t>
   </si>
 </sst>
 </file>
@@ -1126,11 +1135,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D97DC75-4AFF-4124-947F-DBD8EE548F59}">
-  <dimension ref="A1:E158"/>
+  <dimension ref="A1:E160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B158" sqref="B158"/>
+      <selection pane="bottomLeft" activeCell="C160" sqref="C160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3813,7 +3822,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>220</v>
@@ -3825,6 +3834,40 @@
         <v>28</v>
       </c>
       <c r="E158" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="3">
+        <v>158</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E159" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="3">
+        <v>159</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E160" s="4" t="s">
         <v>222</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: correct gene names
</commit_message>
<xml_diff>
--- a/data/manual/manual_gene-list.xlsx
+++ b/data/manual/manual_gene-list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8909B715-F61A-4CF8-97AA-06E594AB081F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF3FF8E-4D9D-48AE-86AE-5F3215D9440F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C95C6FED-A9B1-47B9-B1E7-71E7CD4356DD}"/>
   </bookViews>
@@ -705,13 +705,13 @@
     <t>2025-09-10</t>
   </si>
   <si>
-    <t>MRE11A</t>
-  </si>
-  <si>
-    <t>FAM175A</t>
-  </si>
-  <si>
     <t>TruRisk v5.0 Genpanel research gene</t>
+  </si>
+  <si>
+    <t>MRE11</t>
+  </si>
+  <si>
+    <t>ABRAXAS1</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1139,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C160" sqref="C160"/>
+      <selection pane="bottomLeft" activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3842,10 +3842,10 @@
         <v>158</v>
       </c>
       <c r="B159" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C159" s="3" t="s">
         <v>223</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>225</v>
       </c>
       <c r="D159" s="3" t="s">
         <v>28</v>
@@ -3859,10 +3859,10 @@
         <v>159</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>28</v>

</xml_diff>